<commit_message>
WSBD ready to order.
</commit_message>
<xml_diff>
--- a/5_Hardware/WSBD_Board/Project Outputs for WSBD_Board/Bill of Materials/Bill of Materials-WSBD_Board.xlsx
+++ b/5_Hardware/WSBD_Board/Project Outputs for WSBD_Board/Bill of Materials/Bill of Materials-WSBD_Board.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27525"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fe2074dc24c052ba/Beruflich/TBZ/Projects/Wireless-ScoreBoard-Display/5_Hardware/WSBD_Board/Project Outputs for WSBD_Board/Bill of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FEB1111-DBBB-4A3F-819E-7CCA800FCC48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57B48ACA-8B18-47B7-97E8-95D7507C7675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="16230" xr2:uid="{ACF37913-8D5A-427E-A08A-C7F3EF7DEB6B}"/>
+    <workbookView xWindow="3360" yWindow="3360" windowWidth="23040" windowHeight="12120" xr2:uid="{1B219120-872A-4A34-BC8B-E5735982C4D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WSBD_Board" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,21 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Bill of Materials-WSBD_Board'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -559,11 +570,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -633,7 +644,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -643,39 +654,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -727,7 +738,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -838,13 +849,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -853,6 +857,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -917,28 +928,48 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00797661-7D26-4757-89A1-60FDDCB31BEB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DF6C82-E75C-44F3-92F9-64EF6A04028B}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="10" width="20" customWidth="1"/>
+    <col min="1" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -970,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1034,7 +1065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +1097,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1193,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
@@ -1258,7 +1289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1290,7 +1321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1410,7 +1441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
@@ -1442,7 +1473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
@@ -1506,7 +1537,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1602,7 +1633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -1634,7 +1665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -1666,7 +1697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>0</v>
       </c>
@@ -1698,7 +1729,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
@@ -1760,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1790,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>0</v>
       </c>
@@ -1850,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>0</v>
       </c>
@@ -1882,7 +1913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
         <v>0</v>
       </c>
@@ -1914,7 +1945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +1976,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>